<commit_message>
chore: update NOFO docs
</commit_message>
<xml_diff>
--- a/static/grants/20181102rsatmat/RSATBudget2018.xlsx
+++ b/static/grants/20181102rsatmat/RSATBudget2018.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgleicher\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\RSAT Work group\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="941"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17925" windowHeight="9510" tabRatio="941"/>
   </bookViews>
   <sheets>
     <sheet name="Section A - ICJIA Funds" sheetId="1" r:id="rId1"/>
@@ -3294,9 +3294,6 @@
     <t xml:space="preserve">DUNS#:  </t>
   </si>
   <si>
-    <t xml:space="preserve">NOFO ID: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Grant #: </t>
   </si>
   <si>
@@ -3749,7 +3746,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>2019-2020</t>
+      <t>2018 - 19</t>
     </r>
   </si>
   <si>
@@ -3764,49 +3761,20 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>1/1/2019 - 12/31/2019</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CFSA Number: 
+      <t>03/01/2019 - 02/29/2020</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CSFA Number: 546-00-1740
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>FFY15: 546-00-1401; FFY16: 546-00-1486; FFY17: 546-00-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CSFA Short Description: 
+  </si>
+  <si>
+    <t xml:space="preserve">CSFA Short Description: 
+Residential Substance Abuse Treatment Act (RSAT) FFY18
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Violence Against Women Act (VAWA) FFY15; FFY16; FFY17</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
+  </si>
+  <si>
+    <t>NOFO ID: 1740-636</t>
   </si>
 </sst>
 </file>
@@ -9853,7 +9821,7 @@
   <dimension ref="A1:G130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9889,26 +9857,26 @@
       </c>
       <c r="D2" s="428"/>
       <c r="E2" s="422" t="s">
+        <v>334</v>
+      </c>
+      <c r="F2" s="194" t="s">
         <v>293</v>
-      </c>
-      <c r="F2" s="194" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="429" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B3" s="429"/>
       <c r="C3" s="429" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D3" s="429"/>
       <c r="E3" s="422" t="s">
+        <v>330</v>
+      </c>
+      <c r="F3" s="422" t="s">
         <v>331</v>
-      </c>
-      <c r="F3" s="422" t="s">
-        <v>332</v>
       </c>
       <c r="G3" s="161"/>
     </row>
@@ -10354,7 +10322,7 @@
     </row>
     <row r="29" spans="1:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="447" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B29" s="448"/>
       <c r="C29" s="342">
@@ -14781,11 +14749,11 @@
       <c r="E27" s="479"/>
       <c r="F27" s="480"/>
       <c r="G27" s="489" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H27" s="490"/>
       <c r="I27" s="493" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J27" s="493"/>
       <c r="K27" s="494"/>
@@ -14797,11 +14765,11 @@
       <c r="E28" s="479"/>
       <c r="F28" s="480"/>
       <c r="G28" s="491" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H28" s="492"/>
       <c r="I28" s="495" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J28" s="495"/>
       <c r="K28" s="496"/>
@@ -14813,11 +14781,11 @@
       <c r="E29" s="479"/>
       <c r="F29" s="480"/>
       <c r="G29" s="491" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H29" s="492"/>
       <c r="I29" s="497" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J29" s="497"/>
       <c r="K29" s="498"/>
@@ -14829,11 +14797,11 @@
       <c r="E30" s="479"/>
       <c r="F30" s="480"/>
       <c r="G30" s="471" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H30" s="472"/>
       <c r="I30" s="473" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J30" s="473"/>
       <c r="K30" s="474"/>
@@ -16153,7 +16121,7 @@
     </row>
     <row r="3" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="660" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B3" s="660"/>
       <c r="C3" s="660"/>
@@ -16554,7 +16522,7 @@
       <c r="D2" s="757"/>
       <c r="E2" s="184" t="str">
         <f>'Section A - ICJIA Funds'!E2</f>
-        <v xml:space="preserve">NOFO ID: </v>
+        <v>NOFO ID: 1740-636</v>
       </c>
       <c r="F2" s="184" t="str">
         <f>'Section A - ICJIA Funds'!F2</f>
@@ -16564,26 +16532,26 @@
     <row r="3" spans="1:9" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="758" t="str">
         <f>'Section A - ICJIA Funds'!A3:B3</f>
-        <v>CFSA Number: 
-FFY15: 546-00-1401; FFY16: 546-00-1486; FFY17: 546-00-</v>
+        <v xml:space="preserve">CSFA Number: 546-00-1740
+</v>
       </c>
       <c r="B3" s="759"/>
       <c r="C3" s="758" t="str">
         <f>'Section A - ICJIA Funds'!C3:D3</f>
         <v xml:space="preserve">CSFA Short Description: 
-Violence Against Women Act (VAWA) FFY15; FFY16; FFY17
+Residential Substance Abuse Treatment Act (RSAT) FFY18
 </v>
       </c>
       <c r="D3" s="759"/>
       <c r="E3" s="184" t="str">
         <f>'Section A - ICJIA Funds'!E3</f>
         <v>State Fiscal Year(s): 
-2019-2020</v>
+2018 - 19</v>
       </c>
       <c r="F3" s="184" t="str">
         <f>'Section A - ICJIA Funds'!F3</f>
         <v>Project Period:  
-1/1/2019 - 12/31/2019</v>
+03/01/2019 - 02/29/2020</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -16632,7 +16600,7 @@
     </row>
     <row r="8" spans="1:9" s="404" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="402" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B8" s="749" t="s">
         <v>236</v>
@@ -16656,7 +16624,7 @@
     </row>
     <row r="10" spans="1:9" s="404" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="407" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B10" s="740" t="s">
         <v>239</v>
@@ -16706,7 +16674,7 @@
     </row>
     <row r="15" spans="1:9" s="404" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="402" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B15" s="749" t="s">
         <v>236</v>
@@ -16730,7 +16698,7 @@
     </row>
     <row r="17" spans="1:14" s="404" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="407" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B17" s="740" t="s">
         <v>239</v>
@@ -16772,7 +16740,7 @@
     </row>
     <row r="21" spans="1:14" s="404" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="402" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B21" s="749" t="s">
         <v>236</v>
@@ -16796,7 +16764,7 @@
     </row>
     <row r="23" spans="1:14" s="414" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="407" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B23" s="746" t="s">
         <v>239</v>
@@ -18759,7 +18727,7 @@
     </row>
     <row r="5" spans="2:16" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="464" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C5" s="464"/>
       <c r="D5" s="464"/>
@@ -18816,7 +18784,7 @@
     </row>
     <row r="11" spans="2:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="464" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C11" s="464"/>
       <c r="D11" s="464"/>
@@ -18835,7 +18803,7 @@
     </row>
     <row r="13" spans="2:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="771" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C13" s="771"/>
       <c r="D13" s="771"/>
@@ -19104,7 +19072,7 @@
       <c r="D2" s="504"/>
       <c r="E2" s="202" t="str">
         <f>'Section A - ICJIA Funds'!E2</f>
-        <v xml:space="preserve">NOFO ID: </v>
+        <v>NOFO ID: 1740-636</v>
       </c>
       <c r="F2" s="202" t="str">
         <f>'Section A - ICJIA Funds'!F2</f>
@@ -19114,26 +19082,26 @@
     <row r="3" spans="1:12" ht="42.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="499" t="str">
         <f>'Section A - ICJIA Funds'!A3:B3</f>
-        <v>CFSA Number: 
-FFY15: 546-00-1401; FFY16: 546-00-1486; FFY17: 546-00-</v>
+        <v xml:space="preserve">CSFA Number: 546-00-1740
+</v>
       </c>
       <c r="B3" s="500"/>
       <c r="C3" s="499" t="str">
         <f>'Section A - ICJIA Funds'!C3:D3</f>
         <v xml:space="preserve">CSFA Short Description: 
-Violence Against Women Act (VAWA) FFY15; FFY16; FFY17
+Residential Substance Abuse Treatment Act (RSAT) FFY18
 </v>
       </c>
       <c r="D3" s="500"/>
       <c r="E3" s="202" t="str">
         <f>'Section A - ICJIA Funds'!E3</f>
         <v>State Fiscal Year(s): 
-2019-2020</v>
+2018 - 19</v>
       </c>
       <c r="F3" s="202" t="str">
         <f>'Section A - ICJIA Funds'!F3</f>
         <v>Project Period:  
-1/1/2019 - 12/31/2019</v>
+03/01/2019 - 02/29/2020</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="41.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -19178,7 +19146,7 @@
     </row>
     <row r="7" spans="1:12" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="514" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B7" s="515"/>
       <c r="C7" s="324"/>
@@ -19799,7 +19767,7 @@
       <c r="E2" s="536"/>
       <c r="F2" s="421" t="str">
         <f>'Section A - ICJIA Funds'!E2</f>
-        <v xml:space="preserve">NOFO ID: </v>
+        <v>NOFO ID: 1740-636</v>
       </c>
       <c r="G2" s="541" t="str">
         <f>'Section A - ICJIA Funds'!F2</f>
@@ -19810,14 +19778,14 @@
     <row r="3" spans="1:11" ht="69" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="529" t="str">
         <f>'Section A - ICJIA Funds'!A3:B3</f>
-        <v>CFSA Number: 
-FFY15: 546-00-1401; FFY16: 546-00-1486; FFY17: 546-00-</v>
+        <v xml:space="preserve">CSFA Number: 546-00-1740
+</v>
       </c>
       <c r="B3" s="531"/>
       <c r="C3" s="529" t="str">
         <f>'Section A - ICJIA Funds'!C3:D3</f>
         <v xml:space="preserve">CSFA Short Description: 
-Violence Against Women Act (VAWA) FFY15; FFY16; FFY17
+Residential Substance Abuse Treatment Act (RSAT) FFY18
 </v>
       </c>
       <c r="D3" s="530"/>
@@ -19825,12 +19793,12 @@
       <c r="F3" s="421" t="str">
         <f>'Section A - ICJIA Funds'!E3</f>
         <v>State Fiscal Year(s): 
-2019-2020</v>
+2018 - 19</v>
       </c>
       <c r="G3" s="543" t="str">
         <f>'Section A - ICJIA Funds'!F3</f>
         <v>Project Period:  
-1/1/2019 - 12/31/2019</v>
+03/01/2019 - 02/29/2020</v>
       </c>
       <c r="H3" s="544"/>
     </row>
@@ -19870,7 +19838,7 @@
     </row>
     <row r="8" spans="1:11" s="383" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="546" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B8" s="546"/>
       <c r="C8" s="546"/>
@@ -19879,7 +19847,7 @@
       <c r="F8" s="546"/>
       <c r="G8" s="387"/>
       <c r="H8" s="390" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I8" s="390"/>
       <c r="K8" s="9"/>
@@ -19910,31 +19878,31 @@
     </row>
     <row r="11" spans="1:11" s="383" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="527" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B11" s="527"/>
       <c r="C11" s="359"/>
       <c r="D11" s="359"/>
       <c r="E11" s="526" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F11" s="526"/>
       <c r="G11" s="391"/>
       <c r="H11" s="526" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I11" s="526"/>
       <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" s="383" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="360" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B12" s="359"/>
       <c r="C12" s="359"/>
       <c r="D12" s="359"/>
       <c r="E12" s="393" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F12" s="396"/>
       <c r="G12" s="6"/>
@@ -19957,18 +19925,18 @@
     </row>
     <row r="14" spans="1:11" s="383" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="527" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B14" s="527"/>
       <c r="C14" s="359"/>
       <c r="D14" s="359"/>
       <c r="E14" s="526" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F14" s="526"/>
       <c r="G14" s="391"/>
       <c r="H14" s="526" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I14" s="526"/>
       <c r="K14" s="9"/>
@@ -20004,18 +19972,18 @@
     </row>
     <row r="17" spans="1:11" s="383" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="527" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B17" s="527"/>
       <c r="C17" s="359"/>
       <c r="D17" s="359"/>
       <c r="E17" s="526" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F17" s="526"/>
       <c r="G17" s="391"/>
       <c r="H17" s="526" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I17" s="526"/>
       <c r="K17" s="9"/>
@@ -20051,18 +20019,18 @@
     </row>
     <row r="20" spans="1:11" s="383" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="527" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B20" s="527"/>
       <c r="C20" s="359"/>
       <c r="D20" s="359"/>
       <c r="E20" s="526" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F20" s="526"/>
       <c r="G20" s="391"/>
       <c r="H20" s="526" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I20" s="526"/>
       <c r="K20" s="9"/>
@@ -20113,18 +20081,18 @@
     </row>
     <row r="24" spans="1:11" s="383" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="527" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B24" s="527"/>
       <c r="C24" s="361"/>
       <c r="D24" s="361"/>
       <c r="E24" s="526" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F24" s="526"/>
       <c r="G24" s="391"/>
       <c r="H24" s="545" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I24" s="545"/>
       <c r="J24" s="389"/>
@@ -20323,7 +20291,7 @@
     </row>
     <row r="3" spans="2:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="628" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C3" s="628"/>
       <c r="D3" s="628"/>
@@ -20361,7 +20329,7 @@
     </row>
     <row r="5" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="630" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C5" s="631"/>
       <c r="D5" s="631"/>
@@ -20381,7 +20349,7 @@
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="619" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C6" s="625"/>
       <c r="D6" s="625"/>
@@ -20401,7 +20369,7 @@
     </row>
     <row r="7" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="619" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C7" s="620"/>
       <c r="D7" s="620"/>
@@ -20421,7 +20389,7 @@
     </row>
     <row r="8" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="624" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C8" s="625"/>
       <c r="D8" s="625"/>
@@ -20454,7 +20422,7 @@
       <c r="I9" s="613"/>
       <c r="J9" s="362"/>
       <c r="K9" s="370" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L9" s="363"/>
       <c r="M9" s="562" t="s">
@@ -20467,7 +20435,7 @@
     </row>
     <row r="10" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="609" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C10" s="610"/>
       <c r="D10" s="610"/>
@@ -20500,7 +20468,7 @@
       <c r="I11" s="613"/>
       <c r="J11" s="362"/>
       <c r="K11" s="370" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L11" s="363"/>
       <c r="M11" s="562" t="s">
@@ -20532,7 +20500,7 @@
       <c r="K12" s="615" t="str">
         <f>'Section A - ICJIA Funds'!F3</f>
         <v>Project Period:  
-1/1/2019 - 12/31/2019</v>
+03/01/2019 - 02/29/2020</v>
       </c>
       <c r="L12" s="615"/>
       <c r="M12" s="615"/>
@@ -20543,7 +20511,7 @@
     </row>
     <row r="13" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="582" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C13" s="583"/>
       <c r="D13" s="583"/>
@@ -20565,7 +20533,7 @@
       <c r="B14" s="585" t="str">
         <f>'Section A - ICJIA Funds'!C3</f>
         <v xml:space="preserve">CSFA Short Description: 
-Violence Against Women Act (VAWA) FFY15; FFY16; FFY17
+Residential Substance Abuse Treatment Act (RSAT) FFY18
 </v>
       </c>
       <c r="C14" s="586"/>
@@ -20586,7 +20554,7 @@
     </row>
     <row r="15" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="579" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C15" s="580"/>
       <c r="D15" s="580"/>
@@ -20606,7 +20574,7 @@
     </row>
     <row r="16" spans="2:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="588" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C16" s="589"/>
       <c r="D16" s="589"/>
@@ -20626,7 +20594,7 @@
     </row>
     <row r="17" spans="2:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="591" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C17" s="592"/>
       <c r="D17" s="592"/>
@@ -20684,7 +20652,7 @@
     </row>
     <row r="20" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="600" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C20" s="601"/>
       <c r="D20" s="601"/>
@@ -20722,7 +20690,7 @@
     </row>
     <row r="22" spans="2:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="591" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C22" s="592"/>
       <c r="D22" s="592"/>
@@ -21622,7 +21590,7 @@
     <row r="3" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="660" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C3" s="660"/>
       <c r="D3" s="660"/>
@@ -25457,7 +25425,7 @@
     </row>
     <row r="3" spans="2:13" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="660" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C3" s="660"/>
       <c r="D3" s="660"/>

</xml_diff>